<commit_message>
fix pull down and change tab
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -252,10 +252,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>首页-查询报表-任意一个查询-左上角返回-物理返回-物理返回 null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>000024</t>
-  </si>
-  <si>
-    <t>首页-查询报表-任意一个查询-左上角返回-物理返回-物理返回 null</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -717,7 +718,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1181,10 +1182,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>13</v>

</xml_diff>